<commit_message>
Update columns in exported excel
</commit_message>
<xml_diff>
--- a/edge_research/dataout/18mpip.xlsx
+++ b/edge_research/dataout/18mpip.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>1030_PRICE</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>MAX_PIP_DOWN_1045_DATETIME</t>
+  </si>
+  <si>
+    <t>MAX_PIP_UP_PRIOR_DAY_FIX</t>
+  </si>
+  <si>
+    <t>MAX_PIP_UP_PRIOR_DAY_FIX_DATETIME</t>
+  </si>
+  <si>
+    <t>MAX_PIP_UP_PRIOR_DAY_FIX_PRICE</t>
+  </si>
+  <si>
+    <t>MAX_PIP_DOWN_PRIOR_DAY_FIX</t>
+  </si>
+  <si>
+    <t>MAX_PIP_DOWN_PRIOR_DAY_FIX_DATETIME</t>
+  </si>
+  <si>
+    <t>MAX_PIP_DOWN_PRIOR_DAY_FIX_PRICE</t>
   </si>
 </sst>
 </file>
@@ -421,16 +439,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O260"/>
+  <dimension ref="A1:U260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="15" width="18.7109375" customWidth="1"/>
+    <col min="1" max="21" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,8 +491,26 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="2">
         <v>43102</v>
       </c>
@@ -520,8 +556,14 @@
       <c r="O2" s="3">
         <v>43102.43958333333</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="2">
         <v>43103</v>
       </c>
@@ -567,8 +609,14 @@
       <c r="O3" s="3">
         <v>43103.4375</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="2">
         <v>43104</v>
       </c>
@@ -614,8 +662,14 @@
       <c r="O4" s="3">
         <v>43104.45763888889</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="2">
         <v>43105</v>
       </c>
@@ -661,8 +715,14 @@
       <c r="O5" s="3">
         <v>43105.45069444444</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="2">
         <v>43108</v>
       </c>
@@ -708,8 +768,14 @@
       <c r="O6" s="3">
         <v>43108.44027777778</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="2">
         <v>43109</v>
       </c>
@@ -755,8 +821,14 @@
       <c r="O7" s="3">
         <v>43109.44027777778</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="2">
         <v>43110</v>
       </c>
@@ -802,8 +874,14 @@
       <c r="O8" s="3">
         <v>43110.44722222222</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="2">
         <v>43111</v>
       </c>
@@ -849,8 +927,14 @@
       <c r="O9" s="3">
         <v>43111.4375</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" s="2">
         <v>43112</v>
       </c>
@@ -896,8 +980,14 @@
       <c r="O10" s="3">
         <v>43112.43958333333</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="2">
         <v>43115</v>
       </c>
@@ -943,8 +1033,14 @@
       <c r="O11" s="3">
         <v>43115.44305555556</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="2">
         <v>43116</v>
       </c>
@@ -990,8 +1086,14 @@
       <c r="O12" s="3">
         <v>43116.4375</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="2">
         <v>43117</v>
       </c>
@@ -1037,8 +1139,14 @@
       <c r="O13" s="3">
         <v>43117.44236111111</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="2">
         <v>43118</v>
       </c>
@@ -1084,8 +1192,14 @@
       <c r="O14" s="3">
         <v>43118.44236111111</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="2">
         <v>43119</v>
       </c>
@@ -1131,8 +1245,14 @@
       <c r="O15" s="3">
         <v>43119.45763888889</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="2">
         <v>43122</v>
       </c>
@@ -1178,8 +1298,14 @@
       <c r="O16" s="3">
         <v>43122.4375</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="2">
         <v>43123</v>
       </c>
@@ -1225,8 +1351,14 @@
       <c r="O17" s="3">
         <v>43123.43819444445</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="2">
         <v>43124</v>
       </c>
@@ -1272,8 +1404,14 @@
       <c r="O18" s="3">
         <v>43124.44305555556</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="2">
         <v>43125</v>
       </c>
@@ -1319,8 +1457,14 @@
       <c r="O19" s="3">
         <v>43125.44097222222</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="2">
         <v>43126</v>
       </c>
@@ -1366,8 +1510,14 @@
       <c r="O20" s="3">
         <v>43126.43888888889</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="2">
         <v>43129</v>
       </c>
@@ -1413,8 +1563,14 @@
       <c r="O21" s="3">
         <v>43129.45972222222</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="2">
         <v>43130</v>
       </c>
@@ -1460,8 +1616,14 @@
       <c r="O22" s="3">
         <v>43130.45833333334</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="2">
         <v>43131</v>
       </c>
@@ -1507,8 +1669,14 @@
       <c r="O23" s="3">
         <v>43131.44027777778</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="2">
         <v>43132</v>
       </c>
@@ -1554,8 +1722,14 @@
       <c r="O24" s="3">
         <v>43132.4375</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="2">
         <v>43133</v>
       </c>
@@ -1601,8 +1775,14 @@
       <c r="O25" s="3">
         <v>43133.44930555556</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="2">
         <v>43136</v>
       </c>
@@ -1648,8 +1828,14 @@
       <c r="O26" s="3">
         <v>43136.44652777778</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="2">
         <v>43137</v>
       </c>
@@ -1695,8 +1881,14 @@
       <c r="O27" s="3">
         <v>43137.44166666667</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="2">
         <v>43138</v>
       </c>
@@ -1742,8 +1934,14 @@
       <c r="O28" s="3">
         <v>43138.45972222222</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="2">
         <v>43139</v>
       </c>
@@ -1789,8 +1987,14 @@
       <c r="O29" s="3">
         <v>43139.45972222222</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="2">
         <v>43140</v>
       </c>
@@ -1836,8 +2040,14 @@
       <c r="O30" s="3">
         <v>43140.44513888889</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="2">
         <v>43143</v>
       </c>
@@ -1883,8 +2093,14 @@
       <c r="O31" s="3">
         <v>43143.44791666666</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="2">
         <v>43144</v>
       </c>
@@ -1930,8 +2146,14 @@
       <c r="O32" s="3">
         <v>43144.45902777778</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="2">
         <v>43145</v>
       </c>
@@ -1977,8 +2199,14 @@
       <c r="O33" s="3">
         <v>43145.4375</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="2">
         <v>43146</v>
       </c>
@@ -2024,8 +2252,14 @@
       <c r="O34" s="3">
         <v>43146.44930555556</v>
       </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="2">
         <v>43147</v>
       </c>
@@ -2071,8 +2305,14 @@
       <c r="O35" s="3">
         <v>43147.45694444444</v>
       </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="2">
         <v>43150</v>
       </c>
@@ -2118,8 +2358,14 @@
       <c r="O36" s="3">
         <v>43150.44027777778</v>
       </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="2">
         <v>43151</v>
       </c>
@@ -2165,8 +2411,14 @@
       <c r="O37" s="3">
         <v>43151.43819444445</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="2">
         <v>43152</v>
       </c>
@@ -2212,8 +2464,14 @@
       <c r="O38" s="3">
         <v>43152.45</v>
       </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="2">
         <v>43153</v>
       </c>
@@ -2259,8 +2517,14 @@
       <c r="O39" s="3">
         <v>43153.45277777778</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="2">
         <v>43154</v>
       </c>
@@ -2306,8 +2570,14 @@
       <c r="O40" s="3">
         <v>43154.45694444444</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="2">
         <v>43157</v>
       </c>
@@ -2353,8 +2623,14 @@
       <c r="O41" s="3">
         <v>43157.45555555556</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="2">
         <v>43158</v>
       </c>
@@ -2400,8 +2676,14 @@
       <c r="O42" s="3">
         <v>43158.45486111111</v>
       </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="2">
         <v>43159</v>
       </c>
@@ -2447,8 +2729,14 @@
       <c r="O43" s="3">
         <v>43159.45902777778</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="2">
         <v>43160</v>
       </c>
@@ -2494,8 +2782,14 @@
       <c r="O44" s="3">
         <v>43160.45833333334</v>
       </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="2">
         <v>43161</v>
       </c>
@@ -2541,8 +2835,14 @@
       <c r="O45" s="3">
         <v>43161.45069444444</v>
       </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="2">
         <v>43164</v>
       </c>
@@ -2588,8 +2888,14 @@
       <c r="O46" s="3">
         <v>43164.44097222222</v>
       </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="2">
         <v>43165</v>
       </c>
@@ -2635,8 +2941,14 @@
       <c r="O47" s="3">
         <v>43165.45694444444</v>
       </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="2">
         <v>43166</v>
       </c>
@@ -2682,8 +2994,14 @@
       <c r="O48" s="3">
         <v>43166.4375</v>
       </c>
-    </row>
-    <row r="49" spans="1:15">
+      <c r="P48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="2">
         <v>43167</v>
       </c>
@@ -2729,8 +3047,14 @@
       <c r="O49" s="3">
         <v>43167.45069444444</v>
       </c>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="2">
         <v>43168</v>
       </c>
@@ -2776,8 +3100,14 @@
       <c r="O50" s="3">
         <v>43168.45972222222</v>
       </c>
-    </row>
-    <row r="51" spans="1:15">
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="2">
         <v>43171</v>
       </c>
@@ -2823,8 +3153,14 @@
       <c r="O51" s="3">
         <v>43171.4375</v>
       </c>
-    </row>
-    <row r="52" spans="1:15">
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="S51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="2">
         <v>43172</v>
       </c>
@@ -2870,8 +3206,14 @@
       <c r="O52" s="3">
         <v>43172.43819444445</v>
       </c>
-    </row>
-    <row r="53" spans="1:15">
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="2">
         <v>43173</v>
       </c>
@@ -2917,8 +3259,14 @@
       <c r="O53" s="3">
         <v>43173.43958333333</v>
       </c>
-    </row>
-    <row r="54" spans="1:15">
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="2">
         <v>43174</v>
       </c>
@@ -2964,8 +3312,14 @@
       <c r="O54" s="3">
         <v>43174.43958333333</v>
       </c>
-    </row>
-    <row r="55" spans="1:15">
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="2">
         <v>43175</v>
       </c>
@@ -3011,8 +3365,14 @@
       <c r="O55" s="3">
         <v>43175.45833333334</v>
       </c>
-    </row>
-    <row r="56" spans="1:15">
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="2">
         <v>43178</v>
       </c>
@@ -3058,8 +3418,14 @@
       <c r="O56" s="3">
         <v>43178.45972222222</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="2">
         <v>43179</v>
       </c>
@@ -3105,8 +3471,14 @@
       <c r="O57" s="3">
         <v>43179.4375</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" s="2">
         <v>43180</v>
       </c>
@@ -3152,8 +3524,14 @@
       <c r="O58" s="3">
         <v>43180.44513888889</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" s="2">
         <v>43181</v>
       </c>
@@ -3199,8 +3577,14 @@
       <c r="O59" s="3">
         <v>43181.45208333333</v>
       </c>
-    </row>
-    <row r="60" spans="1:15">
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" s="2">
         <v>43182</v>
       </c>
@@ -3246,8 +3630,14 @@
       <c r="O60" s="3">
         <v>43182.45416666667</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" s="2">
         <v>43185</v>
       </c>
@@ -3293,8 +3683,14 @@
       <c r="O61" s="3">
         <v>43185.4375</v>
       </c>
-    </row>
-    <row r="62" spans="1:15">
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="S61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" s="2">
         <v>43186</v>
       </c>
@@ -3340,8 +3736,14 @@
       <c r="O62" s="3">
         <v>43186.45555555556</v>
       </c>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="P62">
+        <v>0</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" s="2">
         <v>43187</v>
       </c>
@@ -3387,8 +3789,14 @@
       <c r="O63" s="3">
         <v>43187.44583333333</v>
       </c>
-    </row>
-    <row r="64" spans="1:15">
+      <c r="P63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" s="2">
         <v>43188</v>
       </c>
@@ -3434,8 +3842,14 @@
       <c r="O64" s="3">
         <v>43188.45902777778</v>
       </c>
-    </row>
-    <row r="65" spans="1:15">
+      <c r="P64">
+        <v>0</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19">
       <c r="A65" s="2">
         <v>43189</v>
       </c>
@@ -3481,8 +3895,14 @@
       <c r="O65" s="3">
         <v>43189.45972222222</v>
       </c>
-    </row>
-    <row r="66" spans="1:15">
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" s="2">
         <v>43192</v>
       </c>
@@ -3528,8 +3948,14 @@
       <c r="O66" s="3">
         <v>43192.45277777778</v>
       </c>
-    </row>
-    <row r="67" spans="1:15">
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67" s="2">
         <v>43193</v>
       </c>
@@ -3575,8 +4001,14 @@
       <c r="O67" s="3">
         <v>43193.44722222222</v>
       </c>
-    </row>
-    <row r="68" spans="1:15">
+      <c r="P67">
+        <v>0</v>
+      </c>
+      <c r="S67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19">
       <c r="A68" s="2">
         <v>43194</v>
       </c>
@@ -3622,8 +4054,14 @@
       <c r="O68" s="3">
         <v>43194.44861111111</v>
       </c>
-    </row>
-    <row r="69" spans="1:15">
+      <c r="P68">
+        <v>0</v>
+      </c>
+      <c r="S68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69" s="2">
         <v>43195</v>
       </c>
@@ -3669,8 +4107,14 @@
       <c r="O69" s="3">
         <v>43195.45694444444</v>
       </c>
-    </row>
-    <row r="70" spans="1:15">
+      <c r="P69">
+        <v>0</v>
+      </c>
+      <c r="S69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19">
       <c r="A70" s="2">
         <v>43196</v>
       </c>
@@ -3716,8 +4160,14 @@
       <c r="O70" s="3">
         <v>43196.45833333334</v>
       </c>
-    </row>
-    <row r="71" spans="1:15">
+      <c r="P70">
+        <v>0</v>
+      </c>
+      <c r="S70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19">
       <c r="A71" s="2">
         <v>43199</v>
       </c>
@@ -3763,8 +4213,14 @@
       <c r="O71" s="3">
         <v>43199.45902777778</v>
       </c>
-    </row>
-    <row r="72" spans="1:15">
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19">
       <c r="A72" s="2">
         <v>43200</v>
       </c>
@@ -3810,8 +4266,14 @@
       <c r="O72" s="3">
         <v>43200.45625</v>
       </c>
-    </row>
-    <row r="73" spans="1:15">
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19">
       <c r="A73" s="2">
         <v>43201</v>
       </c>
@@ -3857,8 +4319,14 @@
       <c r="O73" s="3">
         <v>43201.45763888889</v>
       </c>
-    </row>
-    <row r="74" spans="1:15">
+      <c r="P73">
+        <v>0</v>
+      </c>
+      <c r="S73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19">
       <c r="A74" s="2">
         <v>43202</v>
       </c>
@@ -3904,8 +4372,14 @@
       <c r="O74" s="3">
         <v>43202.44027777778</v>
       </c>
-    </row>
-    <row r="75" spans="1:15">
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="S74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19">
       <c r="A75" s="2">
         <v>43203</v>
       </c>
@@ -3951,8 +4425,14 @@
       <c r="O75" s="3">
         <v>43203.45902777778</v>
       </c>
-    </row>
-    <row r="76" spans="1:15">
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19">
       <c r="A76" s="2">
         <v>43206</v>
       </c>
@@ -3998,8 +4478,14 @@
       <c r="O76" s="3">
         <v>43206.44930555556</v>
       </c>
-    </row>
-    <row r="77" spans="1:15">
+      <c r="P76">
+        <v>0</v>
+      </c>
+      <c r="S76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19">
       <c r="A77" s="2">
         <v>43207</v>
       </c>
@@ -4045,8 +4531,14 @@
       <c r="O77" s="3">
         <v>43207.45902777778</v>
       </c>
-    </row>
-    <row r="78" spans="1:15">
+      <c r="P77">
+        <v>0</v>
+      </c>
+      <c r="S77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19">
       <c r="A78" s="2">
         <v>43208</v>
       </c>
@@ -4092,8 +4584,14 @@
       <c r="O78" s="3">
         <v>43208.45486111111</v>
       </c>
-    </row>
-    <row r="79" spans="1:15">
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19">
       <c r="A79" s="2">
         <v>43209</v>
       </c>
@@ -4139,8 +4637,14 @@
       <c r="O79" s="3">
         <v>43209.45694444444</v>
       </c>
-    </row>
-    <row r="80" spans="1:15">
+      <c r="P79">
+        <v>0</v>
+      </c>
+      <c r="S79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19">
       <c r="A80" s="2">
         <v>43210</v>
       </c>
@@ -4186,8 +4690,14 @@
       <c r="O80" s="3">
         <v>43210.43888888889</v>
       </c>
-    </row>
-    <row r="81" spans="1:15">
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" s="2">
         <v>43213</v>
       </c>
@@ -4233,8 +4743,14 @@
       <c r="O81" s="3">
         <v>43213.45138888889</v>
       </c>
-    </row>
-    <row r="82" spans="1:15">
+      <c r="P81">
+        <v>0</v>
+      </c>
+      <c r="S81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:19">
       <c r="A82" s="2">
         <v>43214</v>
       </c>
@@ -4280,8 +4796,14 @@
       <c r="O82" s="3">
         <v>43214.44444444445</v>
       </c>
-    </row>
-    <row r="83" spans="1:15">
+      <c r="P82">
+        <v>0</v>
+      </c>
+      <c r="S82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:19">
       <c r="A83" s="2">
         <v>43215</v>
       </c>
@@ -4327,8 +4849,14 @@
       <c r="O83" s="3">
         <v>43215.44166666667</v>
       </c>
-    </row>
-    <row r="84" spans="1:15">
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="S83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:19">
       <c r="A84" s="2">
         <v>43216</v>
       </c>
@@ -4374,8 +4902,14 @@
       <c r="O84" s="3">
         <v>43216.45972222222</v>
       </c>
-    </row>
-    <row r="85" spans="1:15">
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="S84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19">
       <c r="A85" s="2">
         <v>43217</v>
       </c>
@@ -4421,8 +4955,14 @@
       <c r="O85" s="3">
         <v>43217.4375</v>
       </c>
-    </row>
-    <row r="86" spans="1:15">
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="S85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19">
       <c r="A86" s="2">
         <v>43220</v>
       </c>
@@ -4468,8 +5008,14 @@
       <c r="O86" s="3">
         <v>43220.45486111111</v>
       </c>
-    </row>
-    <row r="87" spans="1:15">
+      <c r="P86">
+        <v>0</v>
+      </c>
+      <c r="S86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19">
       <c r="A87" s="2">
         <v>43221</v>
       </c>
@@ -4515,8 +5061,14 @@
       <c r="O87" s="3">
         <v>43221.45902777778</v>
       </c>
-    </row>
-    <row r="88" spans="1:15">
+      <c r="P87">
+        <v>0</v>
+      </c>
+      <c r="S87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19">
       <c r="A88" s="2">
         <v>43222</v>
       </c>
@@ -4562,8 +5114,14 @@
       <c r="O88" s="3">
         <v>43222.45902777778</v>
       </c>
-    </row>
-    <row r="89" spans="1:15">
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="S88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19">
       <c r="A89" s="2">
         <v>43223</v>
       </c>
@@ -4609,8 +5167,14 @@
       <c r="O89" s="3">
         <v>43223.45902777778</v>
       </c>
-    </row>
-    <row r="90" spans="1:15">
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="S89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19">
       <c r="A90" s="2">
         <v>43224</v>
       </c>
@@ -4656,8 +5220,14 @@
       <c r="O90" s="3">
         <v>43224.4375</v>
       </c>
-    </row>
-    <row r="91" spans="1:15">
+      <c r="P90">
+        <v>0</v>
+      </c>
+      <c r="S90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19">
       <c r="A91" s="2">
         <v>43227</v>
       </c>
@@ -4703,8 +5273,14 @@
       <c r="O91" s="3">
         <v>43227.44513888889</v>
       </c>
-    </row>
-    <row r="92" spans="1:15">
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="S91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19">
       <c r="A92" s="2">
         <v>43228</v>
       </c>
@@ -4750,8 +5326,14 @@
       <c r="O92" s="3">
         <v>43228.4375</v>
       </c>
-    </row>
-    <row r="93" spans="1:15">
+      <c r="P92">
+        <v>0</v>
+      </c>
+      <c r="S92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19">
       <c r="A93" s="2">
         <v>43229</v>
       </c>
@@ -4797,8 +5379,14 @@
       <c r="O93" s="3">
         <v>43229.45694444444</v>
       </c>
-    </row>
-    <row r="94" spans="1:15">
+      <c r="P93">
+        <v>0</v>
+      </c>
+      <c r="S93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19">
       <c r="A94" s="2">
         <v>43230</v>
       </c>
@@ -4844,8 +5432,14 @@
       <c r="O94" s="3">
         <v>43230.45277777778</v>
       </c>
-    </row>
-    <row r="95" spans="1:15">
+      <c r="P94">
+        <v>0</v>
+      </c>
+      <c r="S94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19">
       <c r="A95" s="2">
         <v>43231</v>
       </c>
@@ -4891,8 +5485,14 @@
       <c r="O95" s="3">
         <v>43231.45138888889</v>
       </c>
-    </row>
-    <row r="96" spans="1:15">
+      <c r="P95">
+        <v>0</v>
+      </c>
+      <c r="S95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19">
       <c r="A96" s="2">
         <v>43234</v>
       </c>
@@ -4938,8 +5538,14 @@
       <c r="O96" s="3">
         <v>43234.44166666667</v>
       </c>
-    </row>
-    <row r="97" spans="1:15">
+      <c r="P96">
+        <v>0</v>
+      </c>
+      <c r="S96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19">
       <c r="A97" s="2">
         <v>43235</v>
       </c>
@@ -4985,8 +5591,14 @@
       <c r="O97" s="3">
         <v>43235.44513888889</v>
       </c>
-    </row>
-    <row r="98" spans="1:15">
+      <c r="P97">
+        <v>0</v>
+      </c>
+      <c r="S97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19">
       <c r="A98" s="2">
         <v>43236</v>
       </c>
@@ -5032,8 +5644,14 @@
       <c r="O98" s="3">
         <v>43236.45625</v>
       </c>
-    </row>
-    <row r="99" spans="1:15">
+      <c r="P98">
+        <v>0</v>
+      </c>
+      <c r="S98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:19">
       <c r="A99" s="2">
         <v>43237</v>
       </c>
@@ -5079,8 +5697,14 @@
       <c r="O99" s="3">
         <v>43237.45972222222</v>
       </c>
-    </row>
-    <row r="100" spans="1:15">
+      <c r="P99">
+        <v>0</v>
+      </c>
+      <c r="S99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19">
       <c r="A100" s="2">
         <v>43238</v>
       </c>
@@ -5126,8 +5750,14 @@
       <c r="O100" s="3">
         <v>43238.44097222222</v>
       </c>
-    </row>
-    <row r="101" spans="1:15">
+      <c r="P100">
+        <v>0</v>
+      </c>
+      <c r="S100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19">
       <c r="A101" s="2">
         <v>43241</v>
       </c>
@@ -5173,8 +5803,14 @@
       <c r="O101" s="3">
         <v>43241.45972222222</v>
       </c>
-    </row>
-    <row r="102" spans="1:15">
+      <c r="P101">
+        <v>0</v>
+      </c>
+      <c r="S101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:19">
       <c r="A102" s="2">
         <v>43242</v>
       </c>
@@ -5220,8 +5856,14 @@
       <c r="O102" s="3">
         <v>43242.45138888889</v>
       </c>
-    </row>
-    <row r="103" spans="1:15">
+      <c r="P102">
+        <v>0</v>
+      </c>
+      <c r="S102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19">
       <c r="A103" s="2">
         <v>43243</v>
       </c>
@@ -5267,8 +5909,14 @@
       <c r="O103" s="3">
         <v>43243.45902777778</v>
       </c>
-    </row>
-    <row r="104" spans="1:15">
+      <c r="P103">
+        <v>0</v>
+      </c>
+      <c r="S103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19">
       <c r="A104" s="2">
         <v>43244</v>
       </c>
@@ -5314,8 +5962,14 @@
       <c r="O104" s="3">
         <v>43244.45486111111</v>
       </c>
-    </row>
-    <row r="105" spans="1:15">
+      <c r="P104">
+        <v>0</v>
+      </c>
+      <c r="S104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19">
       <c r="A105" s="2">
         <v>43245</v>
       </c>
@@ -5361,8 +6015,14 @@
       <c r="O105" s="3">
         <v>43245.45347222222</v>
       </c>
-    </row>
-    <row r="106" spans="1:15">
+      <c r="P105">
+        <v>0</v>
+      </c>
+      <c r="S105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19">
       <c r="A106" s="2">
         <v>43248</v>
       </c>
@@ -5408,8 +6068,14 @@
       <c r="O106" s="3">
         <v>43248.45694444444</v>
       </c>
-    </row>
-    <row r="107" spans="1:15">
+      <c r="P106">
+        <v>0</v>
+      </c>
+      <c r="S106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:19">
       <c r="A107" s="2">
         <v>43249</v>
       </c>
@@ -5455,8 +6121,14 @@
       <c r="O107" s="3">
         <v>43249.45972222222</v>
       </c>
-    </row>
-    <row r="108" spans="1:15">
+      <c r="P107">
+        <v>0</v>
+      </c>
+      <c r="S107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:19">
       <c r="A108" s="2">
         <v>43250</v>
       </c>
@@ -5502,8 +6174,14 @@
       <c r="O108" s="3">
         <v>43250.45486111111</v>
       </c>
-    </row>
-    <row r="109" spans="1:15">
+      <c r="P108">
+        <v>0</v>
+      </c>
+      <c r="S108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19">
       <c r="A109" s="2">
         <v>43251</v>
       </c>
@@ -5549,8 +6227,14 @@
       <c r="O109" s="3">
         <v>43251.45972222222</v>
       </c>
-    </row>
-    <row r="110" spans="1:15">
+      <c r="P109">
+        <v>0</v>
+      </c>
+      <c r="S109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19">
       <c r="A110" s="2">
         <v>43252</v>
       </c>
@@ -5596,8 +6280,14 @@
       <c r="O110" s="3">
         <v>43252.44236111111</v>
       </c>
-    </row>
-    <row r="111" spans="1:15">
+      <c r="P110">
+        <v>0</v>
+      </c>
+      <c r="S110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19">
       <c r="A111" s="2">
         <v>43255</v>
       </c>
@@ -5643,8 +6333,14 @@
       <c r="O111" s="3">
         <v>43255.45694444444</v>
       </c>
-    </row>
-    <row r="112" spans="1:15">
+      <c r="P111">
+        <v>0</v>
+      </c>
+      <c r="S111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19">
       <c r="A112" s="2">
         <v>43256</v>
       </c>
@@ -5690,8 +6386,14 @@
       <c r="O112" s="3">
         <v>43256.44166666667</v>
       </c>
-    </row>
-    <row r="113" spans="1:15">
+      <c r="P112">
+        <v>0</v>
+      </c>
+      <c r="S112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19">
       <c r="A113" s="2">
         <v>43257</v>
       </c>
@@ -5737,8 +6439,14 @@
       <c r="O113" s="3">
         <v>43257.44583333333</v>
       </c>
-    </row>
-    <row r="114" spans="1:15">
+      <c r="P113">
+        <v>0</v>
+      </c>
+      <c r="S113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:19">
       <c r="A114" s="2">
         <v>43258</v>
       </c>
@@ -5784,8 +6492,14 @@
       <c r="O114" s="3">
         <v>43258.44513888889</v>
       </c>
-    </row>
-    <row r="115" spans="1:15">
+      <c r="P114">
+        <v>0</v>
+      </c>
+      <c r="S114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19">
       <c r="A115" s="2">
         <v>43259</v>
       </c>
@@ -5831,8 +6545,14 @@
       <c r="O115" s="3">
         <v>43259.45069444444</v>
       </c>
-    </row>
-    <row r="116" spans="1:15">
+      <c r="P115">
+        <v>0</v>
+      </c>
+      <c r="S115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:19">
       <c r="A116" s="2">
         <v>43262</v>
       </c>
@@ -5878,8 +6598,14 @@
       <c r="O116" s="3">
         <v>43262.45763888889</v>
       </c>
-    </row>
-    <row r="117" spans="1:15">
+      <c r="P116">
+        <v>0</v>
+      </c>
+      <c r="S116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:19">
       <c r="A117" s="2">
         <v>43263</v>
       </c>
@@ -5925,8 +6651,14 @@
       <c r="O117" s="3">
         <v>43263.45902777778</v>
       </c>
-    </row>
-    <row r="118" spans="1:15">
+      <c r="P117">
+        <v>0</v>
+      </c>
+      <c r="S117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:19">
       <c r="A118" s="2">
         <v>43264</v>
       </c>
@@ -5972,8 +6704,14 @@
       <c r="O118" s="3">
         <v>43264.44444444445</v>
       </c>
-    </row>
-    <row r="119" spans="1:15">
+      <c r="P118">
+        <v>0</v>
+      </c>
+      <c r="S118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19">
       <c r="A119" s="2">
         <v>43265</v>
       </c>
@@ -6019,8 +6757,14 @@
       <c r="O119" s="3">
         <v>43265.44652777778</v>
       </c>
-    </row>
-    <row r="120" spans="1:15">
+      <c r="P119">
+        <v>0</v>
+      </c>
+      <c r="S119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:19">
       <c r="A120" s="2">
         <v>43266</v>
       </c>
@@ -6066,8 +6810,14 @@
       <c r="O120" s="3">
         <v>43266.44236111111</v>
       </c>
-    </row>
-    <row r="121" spans="1:15">
+      <c r="P120">
+        <v>0</v>
+      </c>
+      <c r="S120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19">
       <c r="A121" s="2">
         <v>43269</v>
       </c>
@@ -6113,8 +6863,14 @@
       <c r="O121" s="3">
         <v>43269.43888888889</v>
       </c>
-    </row>
-    <row r="122" spans="1:15">
+      <c r="P121">
+        <v>0</v>
+      </c>
+      <c r="S121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19">
       <c r="A122" s="2">
         <v>43270</v>
       </c>
@@ -6160,8 +6916,14 @@
       <c r="O122" s="3">
         <v>43270.43888888889</v>
       </c>
-    </row>
-    <row r="123" spans="1:15">
+      <c r="P122">
+        <v>0</v>
+      </c>
+      <c r="S122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:19">
       <c r="A123" s="2">
         <v>43271</v>
       </c>
@@ -6207,8 +6969,14 @@
       <c r="O123" s="3">
         <v>43271.45069444444</v>
       </c>
-    </row>
-    <row r="124" spans="1:15">
+      <c r="P123">
+        <v>0</v>
+      </c>
+      <c r="S123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:19">
       <c r="A124" s="2">
         <v>43272</v>
       </c>
@@ -6254,8 +7022,14 @@
       <c r="O124" s="3">
         <v>43272.43888888889</v>
       </c>
-    </row>
-    <row r="125" spans="1:15">
+      <c r="P124">
+        <v>0</v>
+      </c>
+      <c r="S124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:19">
       <c r="A125" s="2">
         <v>43273</v>
       </c>
@@ -6301,8 +7075,14 @@
       <c r="O125" s="3">
         <v>43273.44583333333</v>
       </c>
-    </row>
-    <row r="126" spans="1:15">
+      <c r="P125">
+        <v>0</v>
+      </c>
+      <c r="S125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:19">
       <c r="A126" s="2">
         <v>43276</v>
       </c>
@@ -6348,8 +7128,14 @@
       <c r="O126" s="3">
         <v>43276.45</v>
       </c>
-    </row>
-    <row r="127" spans="1:15">
+      <c r="P126">
+        <v>0</v>
+      </c>
+      <c r="S126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:19">
       <c r="A127" s="2">
         <v>43277</v>
       </c>
@@ -6395,8 +7181,14 @@
       <c r="O127" s="3">
         <v>43277.4375</v>
       </c>
-    </row>
-    <row r="128" spans="1:15">
+      <c r="P127">
+        <v>0</v>
+      </c>
+      <c r="S127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:19">
       <c r="A128" s="2">
         <v>43278</v>
       </c>
@@ -6442,8 +7234,14 @@
       <c r="O128" s="3">
         <v>43278.45555555556</v>
       </c>
-    </row>
-    <row r="129" spans="1:15">
+      <c r="P128">
+        <v>0</v>
+      </c>
+      <c r="S128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:19">
       <c r="A129" s="2">
         <v>43279</v>
       </c>
@@ -6489,8 +7287,14 @@
       <c r="O129" s="3">
         <v>43279.45416666667</v>
       </c>
-    </row>
-    <row r="130" spans="1:15">
+      <c r="P129">
+        <v>0</v>
+      </c>
+      <c r="S129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19">
       <c r="A130" s="2">
         <v>43280</v>
       </c>
@@ -6536,8 +7340,14 @@
       <c r="O130" s="3">
         <v>43280.44236111111</v>
       </c>
-    </row>
-    <row r="131" spans="1:15">
+      <c r="P130">
+        <v>0</v>
+      </c>
+      <c r="S130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:19">
       <c r="A131" s="2">
         <v>43283</v>
       </c>
@@ -6583,8 +7393,14 @@
       <c r="O131" s="3">
         <v>43283.43819444445</v>
       </c>
-    </row>
-    <row r="132" spans="1:15">
+      <c r="P131">
+        <v>0</v>
+      </c>
+      <c r="S131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:19">
       <c r="A132" s="2">
         <v>43284</v>
       </c>
@@ -6630,8 +7446,14 @@
       <c r="O132" s="3">
         <v>43284.45208333333</v>
       </c>
-    </row>
-    <row r="133" spans="1:15">
+      <c r="P132">
+        <v>0</v>
+      </c>
+      <c r="S132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:19">
       <c r="A133" s="2">
         <v>43285</v>
       </c>
@@ -6677,8 +7499,14 @@
       <c r="O133" s="3">
         <v>43285.45833333334</v>
       </c>
-    </row>
-    <row r="134" spans="1:15">
+      <c r="P133">
+        <v>0</v>
+      </c>
+      <c r="S133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:19">
       <c r="A134" s="2">
         <v>43286</v>
       </c>
@@ -6724,8 +7552,14 @@
       <c r="O134" s="3">
         <v>43286.45486111111</v>
       </c>
-    </row>
-    <row r="135" spans="1:15">
+      <c r="P134">
+        <v>0</v>
+      </c>
+      <c r="S134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:19">
       <c r="A135" s="2">
         <v>43287</v>
       </c>
@@ -6771,8 +7605,14 @@
       <c r="O135" s="3">
         <v>43287.45</v>
       </c>
-    </row>
-    <row r="136" spans="1:15">
+      <c r="P135">
+        <v>0</v>
+      </c>
+      <c r="S135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:19">
       <c r="A136" s="2">
         <v>43290</v>
       </c>
@@ -6818,8 +7658,14 @@
       <c r="O136" s="3">
         <v>43290.4375</v>
       </c>
-    </row>
-    <row r="137" spans="1:15">
+      <c r="P136">
+        <v>0</v>
+      </c>
+      <c r="S136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:19">
       <c r="A137" s="2">
         <v>43291</v>
       </c>
@@ -6865,8 +7711,14 @@
       <c r="O137" s="3">
         <v>43291.44375</v>
       </c>
-    </row>
-    <row r="138" spans="1:15">
+      <c r="P137">
+        <v>0</v>
+      </c>
+      <c r="S137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:19">
       <c r="A138" s="2">
         <v>43292</v>
       </c>
@@ -6912,8 +7764,14 @@
       <c r="O138" s="3">
         <v>43292.45902777778</v>
       </c>
-    </row>
-    <row r="139" spans="1:15">
+      <c r="P138">
+        <v>0</v>
+      </c>
+      <c r="S138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:19">
       <c r="A139" s="2">
         <v>43293</v>
       </c>
@@ -6959,8 +7817,14 @@
       <c r="O139" s="3">
         <v>43293.45138888889</v>
       </c>
-    </row>
-    <row r="140" spans="1:15">
+      <c r="P139">
+        <v>0</v>
+      </c>
+      <c r="S139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:19">
       <c r="A140" s="2">
         <v>43294</v>
       </c>
@@ -7006,8 +7870,14 @@
       <c r="O140" s="3">
         <v>43294.44166666667</v>
       </c>
-    </row>
-    <row r="141" spans="1:15">
+      <c r="P140">
+        <v>0</v>
+      </c>
+      <c r="S140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:19">
       <c r="A141" s="2">
         <v>43297</v>
       </c>
@@ -7053,8 +7923,14 @@
       <c r="O141" s="3">
         <v>43297.45902777778</v>
       </c>
-    </row>
-    <row r="142" spans="1:15">
+      <c r="P141">
+        <v>0</v>
+      </c>
+      <c r="S141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:19">
       <c r="A142" s="2">
         <v>43298</v>
       </c>
@@ -7100,8 +7976,14 @@
       <c r="O142" s="3">
         <v>43298.44097222222</v>
       </c>
-    </row>
-    <row r="143" spans="1:15">
+      <c r="P142">
+        <v>0</v>
+      </c>
+      <c r="S142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:19">
       <c r="A143" s="2">
         <v>43299</v>
       </c>
@@ -7147,8 +8029,14 @@
       <c r="O143" s="3">
         <v>43299.45416666667</v>
       </c>
-    </row>
-    <row r="144" spans="1:15">
+      <c r="P143">
+        <v>0</v>
+      </c>
+      <c r="S143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:19">
       <c r="A144" s="2">
         <v>43300</v>
       </c>
@@ -7194,8 +8082,14 @@
       <c r="O144" s="3">
         <v>43300.44027777778</v>
       </c>
-    </row>
-    <row r="145" spans="1:15">
+      <c r="P144">
+        <v>0</v>
+      </c>
+      <c r="S144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19">
       <c r="A145" s="2">
         <v>43301</v>
       </c>
@@ -7241,8 +8135,14 @@
       <c r="O145" s="3">
         <v>43301.45972222222</v>
       </c>
-    </row>
-    <row r="146" spans="1:15">
+      <c r="P145">
+        <v>0</v>
+      </c>
+      <c r="S145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19">
       <c r="A146" s="2">
         <v>43304</v>
       </c>
@@ -7288,8 +8188,14 @@
       <c r="O146" s="3">
         <v>43304.45625</v>
       </c>
-    </row>
-    <row r="147" spans="1:15">
+      <c r="P146">
+        <v>0</v>
+      </c>
+      <c r="S146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19">
       <c r="A147" s="2">
         <v>43305</v>
       </c>
@@ -7335,8 +8241,14 @@
       <c r="O147" s="3">
         <v>43305.43888888889</v>
       </c>
-    </row>
-    <row r="148" spans="1:15">
+      <c r="P147">
+        <v>0</v>
+      </c>
+      <c r="S147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19">
       <c r="A148" s="2">
         <v>43306</v>
       </c>
@@ -7382,8 +8294,14 @@
       <c r="O148" s="3">
         <v>43306.45555555556</v>
       </c>
-    </row>
-    <row r="149" spans="1:15">
+      <c r="P148">
+        <v>0</v>
+      </c>
+      <c r="S148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19">
       <c r="A149" s="2">
         <v>43307</v>
       </c>
@@ -7429,8 +8347,14 @@
       <c r="O149" s="3">
         <v>43307.43819444445</v>
       </c>
-    </row>
-    <row r="150" spans="1:15">
+      <c r="P149">
+        <v>0</v>
+      </c>
+      <c r="S149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19">
       <c r="A150" s="2">
         <v>43308</v>
       </c>
@@ -7476,8 +8400,14 @@
       <c r="O150" s="3">
         <v>43308.44652777778</v>
       </c>
-    </row>
-    <row r="151" spans="1:15">
+      <c r="P150">
+        <v>0</v>
+      </c>
+      <c r="S150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19">
       <c r="A151" s="2">
         <v>43311</v>
       </c>
@@ -7523,8 +8453,14 @@
       <c r="O151" s="3">
         <v>43311.45833333334</v>
       </c>
-    </row>
-    <row r="152" spans="1:15">
+      <c r="P151">
+        <v>0</v>
+      </c>
+      <c r="S151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19">
       <c r="A152" s="2">
         <v>43312</v>
       </c>
@@ -7570,8 +8506,14 @@
       <c r="O152" s="3">
         <v>43312.45347222222</v>
       </c>
-    </row>
-    <row r="153" spans="1:15">
+      <c r="P152">
+        <v>0</v>
+      </c>
+      <c r="S152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19">
       <c r="A153" s="2">
         <v>43313</v>
       </c>
@@ -7617,8 +8559,14 @@
       <c r="O153" s="3">
         <v>43313.45486111111</v>
       </c>
-    </row>
-    <row r="154" spans="1:15">
+      <c r="P153">
+        <v>0</v>
+      </c>
+      <c r="S153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19">
       <c r="A154" s="2">
         <v>43314</v>
       </c>
@@ -7664,8 +8612,14 @@
       <c r="O154" s="3">
         <v>43314.45694444444</v>
       </c>
-    </row>
-    <row r="155" spans="1:15">
+      <c r="P154">
+        <v>0</v>
+      </c>
+      <c r="S154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:19">
       <c r="A155" s="2">
         <v>43315</v>
       </c>
@@ -7711,8 +8665,14 @@
       <c r="O155" s="3">
         <v>43315.43888888889</v>
       </c>
-    </row>
-    <row r="156" spans="1:15">
+      <c r="P155">
+        <v>0</v>
+      </c>
+      <c r="S155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:19">
       <c r="A156" s="2">
         <v>43318</v>
       </c>
@@ -7758,8 +8718,14 @@
       <c r="O156" s="3">
         <v>43318.45555555556</v>
       </c>
-    </row>
-    <row r="157" spans="1:15">
+      <c r="P156">
+        <v>0</v>
+      </c>
+      <c r="S156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:19">
       <c r="A157" s="2">
         <v>43319</v>
       </c>
@@ -7805,8 +8771,14 @@
       <c r="O157" s="3">
         <v>43319.44722222222</v>
       </c>
-    </row>
-    <row r="158" spans="1:15">
+      <c r="P157">
+        <v>0</v>
+      </c>
+      <c r="S157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:19">
       <c r="A158" s="2">
         <v>43320</v>
       </c>
@@ -7852,8 +8824,14 @@
       <c r="O158" s="3">
         <v>43320.44166666667</v>
       </c>
-    </row>
-    <row r="159" spans="1:15">
+      <c r="P158">
+        <v>0</v>
+      </c>
+      <c r="S158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:19">
       <c r="A159" s="2">
         <v>43321</v>
       </c>
@@ -7899,8 +8877,14 @@
       <c r="O159" s="3">
         <v>43321.45763888889</v>
       </c>
-    </row>
-    <row r="160" spans="1:15">
+      <c r="P159">
+        <v>0</v>
+      </c>
+      <c r="S159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:19">
       <c r="A160" s="2">
         <v>43322</v>
       </c>
@@ -7946,8 +8930,14 @@
       <c r="O160" s="3">
         <v>43322.43888888889</v>
       </c>
-    </row>
-    <row r="161" spans="1:15">
+      <c r="P160">
+        <v>0</v>
+      </c>
+      <c r="S160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19">
       <c r="A161" s="2">
         <v>43325</v>
       </c>
@@ -7993,8 +8983,14 @@
       <c r="O161" s="3">
         <v>43325.45972222222</v>
       </c>
-    </row>
-    <row r="162" spans="1:15">
+      <c r="P161">
+        <v>0</v>
+      </c>
+      <c r="S161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19">
       <c r="A162" s="2">
         <v>43326</v>
       </c>
@@ -8040,8 +9036,14 @@
       <c r="O162" s="3">
         <v>43326.45625</v>
       </c>
-    </row>
-    <row r="163" spans="1:15">
+      <c r="P162">
+        <v>0</v>
+      </c>
+      <c r="S162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:19">
       <c r="A163" s="2">
         <v>43327</v>
       </c>
@@ -8087,8 +9089,14 @@
       <c r="O163" s="3">
         <v>43327.45694444444</v>
       </c>
-    </row>
-    <row r="164" spans="1:15">
+      <c r="P163">
+        <v>0</v>
+      </c>
+      <c r="S163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19">
       <c r="A164" s="2">
         <v>43328</v>
       </c>
@@ -8134,8 +9142,14 @@
       <c r="O164" s="3">
         <v>43328.44930555556</v>
       </c>
-    </row>
-    <row r="165" spans="1:15">
+      <c r="P164">
+        <v>0</v>
+      </c>
+      <c r="S164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:19">
       <c r="A165" s="2">
         <v>43329</v>
       </c>
@@ -8181,8 +9195,14 @@
       <c r="O165" s="3">
         <v>43329.45208333333</v>
       </c>
-    </row>
-    <row r="166" spans="1:15">
+      <c r="P165">
+        <v>0</v>
+      </c>
+      <c r="S165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19">
       <c r="A166" s="2">
         <v>43332</v>
       </c>
@@ -8228,8 +9248,14 @@
       <c r="O166" s="3">
         <v>43332.45833333334</v>
       </c>
-    </row>
-    <row r="167" spans="1:15">
+      <c r="P166">
+        <v>0</v>
+      </c>
+      <c r="S166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19">
       <c r="A167" s="2">
         <v>43333</v>
       </c>
@@ -8275,8 +9301,14 @@
       <c r="O167" s="3">
         <v>43333.45763888889</v>
       </c>
-    </row>
-    <row r="168" spans="1:15">
+      <c r="P167">
+        <v>0</v>
+      </c>
+      <c r="S167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:19">
       <c r="A168" s="2">
         <v>43334</v>
       </c>
@@ -8322,8 +9354,14 @@
       <c r="O168" s="3">
         <v>43334.45347222222</v>
       </c>
-    </row>
-    <row r="169" spans="1:15">
+      <c r="P168">
+        <v>0</v>
+      </c>
+      <c r="S168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:19">
       <c r="A169" s="2">
         <v>43335</v>
       </c>
@@ -8369,8 +9407,14 @@
       <c r="O169" s="3">
         <v>43335.44930555556</v>
       </c>
-    </row>
-    <row r="170" spans="1:15">
+      <c r="P169">
+        <v>0</v>
+      </c>
+      <c r="S169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:19">
       <c r="A170" s="2">
         <v>43336</v>
       </c>
@@ -8416,8 +9460,14 @@
       <c r="O170" s="3">
         <v>43336.44583333333</v>
       </c>
-    </row>
-    <row r="171" spans="1:15">
+      <c r="P170">
+        <v>0</v>
+      </c>
+      <c r="S170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:19">
       <c r="A171" s="2">
         <v>43339</v>
       </c>
@@ -8463,8 +9513,14 @@
       <c r="O171" s="3">
         <v>43339.44444444445</v>
       </c>
-    </row>
-    <row r="172" spans="1:15">
+      <c r="P171">
+        <v>0</v>
+      </c>
+      <c r="S171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:19">
       <c r="A172" s="2">
         <v>43340</v>
       </c>
@@ -8510,8 +9566,14 @@
       <c r="O172" s="3">
         <v>43340.45555555556</v>
       </c>
-    </row>
-    <row r="173" spans="1:15">
+      <c r="P172">
+        <v>0</v>
+      </c>
+      <c r="S172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:19">
       <c r="A173" s="2">
         <v>43341</v>
       </c>
@@ -8557,8 +9619,14 @@
       <c r="O173" s="3">
         <v>43341.44027777778</v>
       </c>
-    </row>
-    <row r="174" spans="1:15">
+      <c r="P173">
+        <v>0</v>
+      </c>
+      <c r="S173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:19">
       <c r="A174" s="2">
         <v>43342</v>
       </c>
@@ -8604,8 +9672,14 @@
       <c r="O174" s="3">
         <v>43342.45833333334</v>
       </c>
-    </row>
-    <row r="175" spans="1:15">
+      <c r="P174">
+        <v>0</v>
+      </c>
+      <c r="S174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:19">
       <c r="A175" s="2">
         <v>43343</v>
       </c>
@@ -8651,8 +9725,14 @@
       <c r="O175" s="3">
         <v>43343.45277777778</v>
       </c>
-    </row>
-    <row r="176" spans="1:15">
+      <c r="P175">
+        <v>0</v>
+      </c>
+      <c r="S175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19">
       <c r="A176" s="2">
         <v>43346</v>
       </c>
@@ -8698,8 +9778,14 @@
       <c r="O176" s="3">
         <v>43346.4375</v>
       </c>
-    </row>
-    <row r="177" spans="1:15">
+      <c r="P176">
+        <v>0</v>
+      </c>
+      <c r="S176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19">
       <c r="A177" s="2">
         <v>43347</v>
       </c>
@@ -8745,8 +9831,14 @@
       <c r="O177" s="3">
         <v>43347.44722222222</v>
       </c>
-    </row>
-    <row r="178" spans="1:15">
+      <c r="P177">
+        <v>0</v>
+      </c>
+      <c r="S177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:19">
       <c r="A178" s="2">
         <v>43348</v>
       </c>
@@ -8792,8 +9884,14 @@
       <c r="O178" s="3">
         <v>43348.45972222222</v>
       </c>
-    </row>
-    <row r="179" spans="1:15">
+      <c r="P178">
+        <v>0</v>
+      </c>
+      <c r="S178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19">
       <c r="A179" s="2">
         <v>43349</v>
       </c>
@@ -8839,8 +9937,14 @@
       <c r="O179" s="3">
         <v>43349.44236111111</v>
       </c>
-    </row>
-    <row r="180" spans="1:15">
+      <c r="P179">
+        <v>0</v>
+      </c>
+      <c r="S179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:19">
       <c r="A180" s="2">
         <v>43350</v>
       </c>
@@ -8886,8 +9990,14 @@
       <c r="O180" s="3">
         <v>43350.45902777778</v>
       </c>
-    </row>
-    <row r="181" spans="1:15">
+      <c r="P180">
+        <v>0</v>
+      </c>
+      <c r="S180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:19">
       <c r="A181" s="2">
         <v>43353</v>
       </c>
@@ -8933,8 +10043,14 @@
       <c r="O181" s="3">
         <v>43353.45069444444</v>
       </c>
-    </row>
-    <row r="182" spans="1:15">
+      <c r="P181">
+        <v>0</v>
+      </c>
+      <c r="S181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19">
       <c r="A182" s="2">
         <v>43354</v>
       </c>
@@ -8980,8 +10096,14 @@
       <c r="O182" s="3">
         <v>43354.44791666666</v>
       </c>
-    </row>
-    <row r="183" spans="1:15">
+      <c r="P182">
+        <v>0</v>
+      </c>
+      <c r="S182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:19">
       <c r="A183" s="2">
         <v>43355</v>
       </c>
@@ -9027,8 +10149,14 @@
       <c r="O183" s="3">
         <v>43355.44375</v>
       </c>
-    </row>
-    <row r="184" spans="1:15">
+      <c r="P183">
+        <v>0</v>
+      </c>
+      <c r="S183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:19">
       <c r="A184" s="2">
         <v>43356</v>
       </c>
@@ -9074,8 +10202,14 @@
       <c r="O184" s="3">
         <v>43356.44652777778</v>
       </c>
-    </row>
-    <row r="185" spans="1:15">
+      <c r="P184">
+        <v>0</v>
+      </c>
+      <c r="S184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:19">
       <c r="A185" s="2">
         <v>43357</v>
       </c>
@@ -9121,8 +10255,14 @@
       <c r="O185" s="3">
         <v>43357.45902777778</v>
       </c>
-    </row>
-    <row r="186" spans="1:15">
+      <c r="P185">
+        <v>0</v>
+      </c>
+      <c r="S185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:19">
       <c r="A186" s="2">
         <v>43360</v>
       </c>
@@ -9168,8 +10308,14 @@
       <c r="O186" s="3">
         <v>43360.45347222222</v>
       </c>
-    </row>
-    <row r="187" spans="1:15">
+      <c r="P186">
+        <v>0</v>
+      </c>
+      <c r="S186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:19">
       <c r="A187" s="2">
         <v>43361</v>
       </c>
@@ -9215,8 +10361,14 @@
       <c r="O187" s="3">
         <v>43361.45625</v>
       </c>
-    </row>
-    <row r="188" spans="1:15">
+      <c r="P187">
+        <v>0</v>
+      </c>
+      <c r="S187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:19">
       <c r="A188" s="2">
         <v>43362</v>
       </c>
@@ -9262,8 +10414,14 @@
       <c r="O188" s="3">
         <v>43362.43819444445</v>
       </c>
-    </row>
-    <row r="189" spans="1:15">
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="S188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:19">
       <c r="A189" s="2">
         <v>43363</v>
       </c>
@@ -9309,8 +10467,14 @@
       <c r="O189" s="3">
         <v>43363.45555555556</v>
       </c>
-    </row>
-    <row r="190" spans="1:15">
+      <c r="P189">
+        <v>0</v>
+      </c>
+      <c r="S189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:19">
       <c r="A190" s="2">
         <v>43364</v>
       </c>
@@ -9356,8 +10520,14 @@
       <c r="O190" s="3">
         <v>43364.4375</v>
       </c>
-    </row>
-    <row r="191" spans="1:15">
+      <c r="P190">
+        <v>0</v>
+      </c>
+      <c r="S190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:19">
       <c r="A191" s="2">
         <v>43367</v>
       </c>
@@ -9403,8 +10573,14 @@
       <c r="O191" s="3">
         <v>43367.44027777778</v>
       </c>
-    </row>
-    <row r="192" spans="1:15">
+      <c r="P191">
+        <v>0</v>
+      </c>
+      <c r="S191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:19">
       <c r="A192" s="2">
         <v>43368</v>
       </c>
@@ -9450,8 +10626,14 @@
       <c r="O192" s="3">
         <v>43368.45</v>
       </c>
-    </row>
-    <row r="193" spans="1:15">
+      <c r="P192">
+        <v>0</v>
+      </c>
+      <c r="S192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:19">
       <c r="A193" s="2">
         <v>43369</v>
       </c>
@@ -9497,8 +10679,14 @@
       <c r="O193" s="3">
         <v>43369.44236111111</v>
       </c>
-    </row>
-    <row r="194" spans="1:15">
+      <c r="P193">
+        <v>0</v>
+      </c>
+      <c r="S193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:19">
       <c r="A194" s="2">
         <v>43370</v>
       </c>
@@ -9544,8 +10732,14 @@
       <c r="O194" s="3">
         <v>43370.45902777778</v>
       </c>
-    </row>
-    <row r="195" spans="1:15">
+      <c r="P194">
+        <v>0</v>
+      </c>
+      <c r="S194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:19">
       <c r="A195" s="2">
         <v>43371</v>
       </c>
@@ -9591,8 +10785,14 @@
       <c r="O195" s="3">
         <v>43371.43888888889</v>
       </c>
-    </row>
-    <row r="196" spans="1:15">
+      <c r="P195">
+        <v>0</v>
+      </c>
+      <c r="S195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:19">
       <c r="A196" s="2">
         <v>43374</v>
       </c>
@@ -9638,8 +10838,14 @@
       <c r="O196" s="3">
         <v>43374.45763888889</v>
       </c>
-    </row>
-    <row r="197" spans="1:15">
+      <c r="P196">
+        <v>0</v>
+      </c>
+      <c r="S196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:19">
       <c r="A197" s="2">
         <v>43375</v>
       </c>
@@ -9685,8 +10891,14 @@
       <c r="O197" s="3">
         <v>43375.44930555556</v>
       </c>
-    </row>
-    <row r="198" spans="1:15">
+      <c r="P197">
+        <v>0</v>
+      </c>
+      <c r="S197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:19">
       <c r="A198" s="2">
         <v>43376</v>
       </c>
@@ -9732,8 +10944,14 @@
       <c r="O198" s="3">
         <v>43376.44652777778</v>
       </c>
-    </row>
-    <row r="199" spans="1:15">
+      <c r="P198">
+        <v>0</v>
+      </c>
+      <c r="S198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:19">
       <c r="A199" s="2">
         <v>43377</v>
       </c>
@@ -9779,8 +10997,14 @@
       <c r="O199" s="3">
         <v>43377.45694444444</v>
       </c>
-    </row>
-    <row r="200" spans="1:15">
+      <c r="P199">
+        <v>0</v>
+      </c>
+      <c r="S199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:19">
       <c r="A200" s="2">
         <v>43378</v>
       </c>
@@ -9826,8 +11050,14 @@
       <c r="O200" s="3">
         <v>43378.44305555556</v>
       </c>
-    </row>
-    <row r="201" spans="1:15">
+      <c r="P200">
+        <v>0</v>
+      </c>
+      <c r="S200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:19">
       <c r="A201" s="2">
         <v>43381</v>
       </c>
@@ -9873,8 +11103,14 @@
       <c r="O201" s="3">
         <v>43381.44375</v>
       </c>
-    </row>
-    <row r="202" spans="1:15">
+      <c r="P201">
+        <v>0</v>
+      </c>
+      <c r="S201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:19">
       <c r="A202" s="2">
         <v>43382</v>
       </c>
@@ -9920,8 +11156,14 @@
       <c r="O202" s="3">
         <v>43382.45972222222</v>
       </c>
-    </row>
-    <row r="203" spans="1:15">
+      <c r="P202">
+        <v>0</v>
+      </c>
+      <c r="S202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:19">
       <c r="A203" s="2">
         <v>43383</v>
       </c>
@@ -9967,8 +11209,14 @@
       <c r="O203" s="3">
         <v>43383.4375</v>
       </c>
-    </row>
-    <row r="204" spans="1:15">
+      <c r="P203">
+        <v>0</v>
+      </c>
+      <c r="S203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:19">
       <c r="A204" s="2">
         <v>43384</v>
       </c>
@@ -10014,8 +11262,14 @@
       <c r="O204" s="3">
         <v>43384.45972222222</v>
       </c>
-    </row>
-    <row r="205" spans="1:15">
+      <c r="P204">
+        <v>0</v>
+      </c>
+      <c r="S204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:19">
       <c r="A205" s="2">
         <v>43385</v>
       </c>
@@ -10061,8 +11315,14 @@
       <c r="O205" s="3">
         <v>43385.45486111111</v>
       </c>
-    </row>
-    <row r="206" spans="1:15">
+      <c r="P205">
+        <v>0</v>
+      </c>
+      <c r="S205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:19">
       <c r="A206" s="2">
         <v>43388</v>
       </c>
@@ -10108,8 +11368,14 @@
       <c r="O206" s="3">
         <v>43388.44027777778</v>
       </c>
-    </row>
-    <row r="207" spans="1:15">
+      <c r="P206">
+        <v>0</v>
+      </c>
+      <c r="S206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:19">
       <c r="A207" s="2">
         <v>43389</v>
       </c>
@@ -10155,8 +11421,14 @@
       <c r="O207" s="3">
         <v>43389.45902777778</v>
       </c>
-    </row>
-    <row r="208" spans="1:15">
+      <c r="P207">
+        <v>0</v>
+      </c>
+      <c r="S207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:19">
       <c r="A208" s="2">
         <v>43390</v>
       </c>
@@ -10202,8 +11474,14 @@
       <c r="O208" s="3">
         <v>43390.45486111111</v>
       </c>
-    </row>
-    <row r="209" spans="1:15">
+      <c r="P208">
+        <v>0</v>
+      </c>
+      <c r="S208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:19">
       <c r="A209" s="2">
         <v>43391</v>
       </c>
@@ -10249,8 +11527,14 @@
       <c r="O209" s="3">
         <v>43391.45486111111</v>
       </c>
-    </row>
-    <row r="210" spans="1:15">
+      <c r="P209">
+        <v>0</v>
+      </c>
+      <c r="S209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:19">
       <c r="A210" s="2">
         <v>43392</v>
       </c>
@@ -10296,8 +11580,14 @@
       <c r="O210" s="3">
         <v>43392.44930555556</v>
       </c>
-    </row>
-    <row r="211" spans="1:15">
+      <c r="P210">
+        <v>0</v>
+      </c>
+      <c r="S210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:19">
       <c r="A211" s="2">
         <v>43395</v>
       </c>
@@ -10343,8 +11633,14 @@
       <c r="O211" s="3">
         <v>43395.45902777778</v>
       </c>
-    </row>
-    <row r="212" spans="1:15">
+      <c r="P211">
+        <v>0</v>
+      </c>
+      <c r="S211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:19">
       <c r="A212" s="2">
         <v>43396</v>
       </c>
@@ -10390,8 +11686,14 @@
       <c r="O212" s="3">
         <v>43396.45902777778</v>
       </c>
-    </row>
-    <row r="213" spans="1:15">
+      <c r="P212">
+        <v>0</v>
+      </c>
+      <c r="S212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19">
       <c r="A213" s="2">
         <v>43397</v>
       </c>
@@ -10437,8 +11739,14 @@
       <c r="O213" s="3">
         <v>43397.45833333334</v>
       </c>
-    </row>
-    <row r="214" spans="1:15">
+      <c r="P213">
+        <v>0</v>
+      </c>
+      <c r="S213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:19">
       <c r="A214" s="2">
         <v>43398</v>
       </c>
@@ -10484,8 +11792,14 @@
       <c r="O214" s="3">
         <v>43398.45972222222</v>
       </c>
-    </row>
-    <row r="215" spans="1:15">
+      <c r="P214">
+        <v>0</v>
+      </c>
+      <c r="S214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:19">
       <c r="A215" s="2">
         <v>43399</v>
       </c>
@@ -10531,8 +11845,14 @@
       <c r="O215" s="3">
         <v>43399.43888888889</v>
       </c>
-    </row>
-    <row r="216" spans="1:15">
+      <c r="P215">
+        <v>0</v>
+      </c>
+      <c r="S215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:19">
       <c r="A216" s="2">
         <v>43402</v>
       </c>
@@ -10578,8 +11898,14 @@
       <c r="O216" s="3">
         <v>43402.4375</v>
       </c>
-    </row>
-    <row r="217" spans="1:15">
+      <c r="P216">
+        <v>0</v>
+      </c>
+      <c r="S216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:19">
       <c r="A217" s="2">
         <v>43403</v>
       </c>
@@ -10625,8 +11951,14 @@
       <c r="O217" s="3">
         <v>43403.45486111111</v>
       </c>
-    </row>
-    <row r="218" spans="1:15">
+      <c r="P217">
+        <v>0</v>
+      </c>
+      <c r="S217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:19">
       <c r="A218" s="2">
         <v>43404</v>
       </c>
@@ -10672,8 +12004,14 @@
       <c r="O218" s="3">
         <v>43404.45486111111</v>
       </c>
-    </row>
-    <row r="219" spans="1:15">
+      <c r="P218">
+        <v>0</v>
+      </c>
+      <c r="S218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:19">
       <c r="A219" s="2">
         <v>43405</v>
       </c>
@@ -10719,8 +12057,14 @@
       <c r="O219" s="3">
         <v>43405.44444444445</v>
       </c>
-    </row>
-    <row r="220" spans="1:15">
+      <c r="P219">
+        <v>0</v>
+      </c>
+      <c r="S219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:19">
       <c r="A220" s="2">
         <v>43406</v>
       </c>
@@ -10766,8 +12110,14 @@
       <c r="O220" s="3">
         <v>43406.45972222222</v>
       </c>
-    </row>
-    <row r="221" spans="1:15">
+      <c r="P220">
+        <v>0</v>
+      </c>
+      <c r="S220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:19">
       <c r="A221" s="2">
         <v>43409</v>
       </c>
@@ -10813,8 +12163,14 @@
       <c r="O221" s="3">
         <v>43409.45069444444</v>
       </c>
-    </row>
-    <row r="222" spans="1:15">
+      <c r="P221">
+        <v>0</v>
+      </c>
+      <c r="S221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:19">
       <c r="A222" s="2">
         <v>43410</v>
       </c>
@@ -10860,8 +12216,14 @@
       <c r="O222" s="3">
         <v>43410.44513888889</v>
       </c>
-    </row>
-    <row r="223" spans="1:15">
+      <c r="P222">
+        <v>0</v>
+      </c>
+      <c r="S222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:19">
       <c r="A223" s="2">
         <v>43411</v>
       </c>
@@ -10907,8 +12269,14 @@
       <c r="O223" s="3">
         <v>43411.45972222222</v>
       </c>
-    </row>
-    <row r="224" spans="1:15">
+      <c r="P223">
+        <v>0</v>
+      </c>
+      <c r="S223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:19">
       <c r="A224" s="2">
         <v>43412</v>
       </c>
@@ -10954,8 +12322,14 @@
       <c r="O224" s="3">
         <v>43412.43958333333</v>
       </c>
-    </row>
-    <row r="225" spans="1:15">
+      <c r="P224">
+        <v>0</v>
+      </c>
+      <c r="S224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:19">
       <c r="A225" s="2">
         <v>43413</v>
       </c>
@@ -11001,8 +12375,14 @@
       <c r="O225" s="3">
         <v>43413.45625</v>
       </c>
-    </row>
-    <row r="226" spans="1:15">
+      <c r="P225">
+        <v>0</v>
+      </c>
+      <c r="S225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:19">
       <c r="A226" s="2">
         <v>43416</v>
       </c>
@@ -11048,8 +12428,14 @@
       <c r="O226" s="3">
         <v>43416.45972222222</v>
       </c>
-    </row>
-    <row r="227" spans="1:15">
+      <c r="P226">
+        <v>0</v>
+      </c>
+      <c r="S226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:19">
       <c r="A227" s="2">
         <v>43417</v>
       </c>
@@ -11095,8 +12481,14 @@
       <c r="O227" s="3">
         <v>43417.44166666667</v>
       </c>
-    </row>
-    <row r="228" spans="1:15">
+      <c r="P227">
+        <v>0</v>
+      </c>
+      <c r="S227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:19">
       <c r="A228" s="2">
         <v>43418</v>
       </c>
@@ -11142,8 +12534,14 @@
       <c r="O228" s="3">
         <v>43418.43958333333</v>
       </c>
-    </row>
-    <row r="229" spans="1:15">
+      <c r="P228">
+        <v>0</v>
+      </c>
+      <c r="S228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:19">
       <c r="A229" s="2">
         <v>43419</v>
       </c>
@@ -11189,8 +12587,14 @@
       <c r="O229" s="3">
         <v>43419.44791666666</v>
       </c>
-    </row>
-    <row r="230" spans="1:15">
+      <c r="P229">
+        <v>0</v>
+      </c>
+      <c r="S229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:19">
       <c r="A230" s="2">
         <v>43420</v>
       </c>
@@ -11236,8 +12640,14 @@
       <c r="O230" s="3">
         <v>43420.45208333333</v>
       </c>
-    </row>
-    <row r="231" spans="1:15">
+      <c r="P230">
+        <v>0</v>
+      </c>
+      <c r="S230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:19">
       <c r="A231" s="2">
         <v>43423</v>
       </c>
@@ -11283,8 +12693,14 @@
       <c r="O231" s="3">
         <v>43423.45902777778</v>
       </c>
-    </row>
-    <row r="232" spans="1:15">
+      <c r="P231">
+        <v>0</v>
+      </c>
+      <c r="S231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:19">
       <c r="A232" s="2">
         <v>43424</v>
       </c>
@@ -11330,8 +12746,14 @@
       <c r="O232" s="3">
         <v>43424.44097222222</v>
       </c>
-    </row>
-    <row r="233" spans="1:15">
+      <c r="P232">
+        <v>0</v>
+      </c>
+      <c r="S232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:19">
       <c r="A233" s="2">
         <v>43425</v>
       </c>
@@ -11377,8 +12799,14 @@
       <c r="O233" s="3">
         <v>43425.45972222222</v>
       </c>
-    </row>
-    <row r="234" spans="1:15">
+      <c r="P233">
+        <v>0</v>
+      </c>
+      <c r="S233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:19">
       <c r="A234" s="2">
         <v>43426</v>
       </c>
@@ -11424,8 +12852,14 @@
       <c r="O234" s="3">
         <v>43426.45416666667</v>
       </c>
-    </row>
-    <row r="235" spans="1:15">
+      <c r="P234">
+        <v>0</v>
+      </c>
+      <c r="S234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:19">
       <c r="A235" s="2">
         <v>43427</v>
       </c>
@@ -11471,8 +12905,14 @@
       <c r="O235" s="3">
         <v>43427.45833333334</v>
       </c>
-    </row>
-    <row r="236" spans="1:15">
+      <c r="P235">
+        <v>0</v>
+      </c>
+      <c r="S235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:19">
       <c r="A236" s="2">
         <v>43430</v>
       </c>
@@ -11518,8 +12958,14 @@
       <c r="O236" s="3">
         <v>43430.45902777778</v>
       </c>
-    </row>
-    <row r="237" spans="1:15">
+      <c r="P236">
+        <v>0</v>
+      </c>
+      <c r="S236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:19">
       <c r="A237" s="2">
         <v>43431</v>
       </c>
@@ -11565,8 +13011,14 @@
       <c r="O237" s="3">
         <v>43431.45972222222</v>
       </c>
-    </row>
-    <row r="238" spans="1:15">
+      <c r="P237">
+        <v>0</v>
+      </c>
+      <c r="S237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:19">
       <c r="A238" s="2">
         <v>43432</v>
       </c>
@@ -11612,8 +13064,14 @@
       <c r="O238" s="3">
         <v>43432.45555555556</v>
       </c>
-    </row>
-    <row r="239" spans="1:15">
+      <c r="P238">
+        <v>0</v>
+      </c>
+      <c r="S238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:19">
       <c r="A239" s="2">
         <v>43433</v>
       </c>
@@ -11659,8 +13117,14 @@
       <c r="O239" s="3">
         <v>43433.45416666667</v>
       </c>
-    </row>
-    <row r="240" spans="1:15">
+      <c r="P239">
+        <v>0</v>
+      </c>
+      <c r="S239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:19">
       <c r="A240" s="2">
         <v>43434</v>
       </c>
@@ -11706,8 +13170,14 @@
       <c r="O240" s="3">
         <v>43434.44097222222</v>
       </c>
-    </row>
-    <row r="241" spans="1:15">
+      <c r="P240">
+        <v>0</v>
+      </c>
+      <c r="S240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:19">
       <c r="A241" s="2">
         <v>43437</v>
       </c>
@@ -11753,8 +13223,14 @@
       <c r="O241" s="3">
         <v>43437.4375</v>
       </c>
-    </row>
-    <row r="242" spans="1:15">
+      <c r="P241">
+        <v>0</v>
+      </c>
+      <c r="S241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:19">
       <c r="A242" s="2">
         <v>43438</v>
       </c>
@@ -11800,8 +13276,14 @@
       <c r="O242" s="3">
         <v>43438.45347222222</v>
       </c>
-    </row>
-    <row r="243" spans="1:15">
+      <c r="P242">
+        <v>0</v>
+      </c>
+      <c r="S242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:19">
       <c r="A243" s="2">
         <v>43439</v>
       </c>
@@ -11847,8 +13329,14 @@
       <c r="O243" s="3">
         <v>43439.44166666667</v>
       </c>
-    </row>
-    <row r="244" spans="1:15">
+      <c r="P243">
+        <v>0</v>
+      </c>
+      <c r="S243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:19">
       <c r="A244" s="2">
         <v>43440</v>
       </c>
@@ -11894,8 +13382,14 @@
       <c r="O244" s="3">
         <v>43440.45625</v>
       </c>
-    </row>
-    <row r="245" spans="1:15">
+      <c r="P244">
+        <v>0</v>
+      </c>
+      <c r="S244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:19">
       <c r="A245" s="2">
         <v>43441</v>
       </c>
@@ -11941,8 +13435,14 @@
       <c r="O245" s="3">
         <v>43441.43888888889</v>
       </c>
-    </row>
-    <row r="246" spans="1:15">
+      <c r="P245">
+        <v>0</v>
+      </c>
+      <c r="S245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:19">
       <c r="A246" s="2">
         <v>43444</v>
       </c>
@@ -11988,8 +13488,14 @@
       <c r="O246" s="3">
         <v>43444.45763888889</v>
       </c>
-    </row>
-    <row r="247" spans="1:15">
+      <c r="P246">
+        <v>0</v>
+      </c>
+      <c r="S246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:19">
       <c r="A247" s="2">
         <v>43445</v>
       </c>
@@ -12035,8 +13541,14 @@
       <c r="O247" s="3">
         <v>43445.45902777778</v>
       </c>
-    </row>
-    <row r="248" spans="1:15">
+      <c r="P247">
+        <v>0</v>
+      </c>
+      <c r="S247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:19">
       <c r="A248" s="2">
         <v>43446</v>
       </c>
@@ -12082,8 +13594,14 @@
       <c r="O248" s="3">
         <v>43446.44722222222</v>
       </c>
-    </row>
-    <row r="249" spans="1:15">
+      <c r="P248">
+        <v>0</v>
+      </c>
+      <c r="S248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:19">
       <c r="A249" s="2">
         <v>43447</v>
       </c>
@@ -12129,8 +13647,14 @@
       <c r="O249" s="3">
         <v>43447.45833333334</v>
       </c>
-    </row>
-    <row r="250" spans="1:15">
+      <c r="P249">
+        <v>0</v>
+      </c>
+      <c r="S249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:19">
       <c r="A250" s="2">
         <v>43448</v>
       </c>
@@ -12176,8 +13700,14 @@
       <c r="O250" s="3">
         <v>43448.4375</v>
       </c>
-    </row>
-    <row r="251" spans="1:15">
+      <c r="P250">
+        <v>0</v>
+      </c>
+      <c r="S250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:19">
       <c r="A251" s="2">
         <v>43451</v>
       </c>
@@ -12223,8 +13753,14 @@
       <c r="O251" s="3">
         <v>43451.45138888889</v>
       </c>
-    </row>
-    <row r="252" spans="1:15">
+      <c r="P251">
+        <v>0</v>
+      </c>
+      <c r="S251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:19">
       <c r="A252" s="2">
         <v>43452</v>
       </c>
@@ -12270,8 +13806,14 @@
       <c r="O252" s="3">
         <v>43452.45763888889</v>
       </c>
-    </row>
-    <row r="253" spans="1:15">
+      <c r="P252">
+        <v>0</v>
+      </c>
+      <c r="S252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:19">
       <c r="A253" s="2">
         <v>43453</v>
       </c>
@@ -12317,8 +13859,14 @@
       <c r="O253" s="3">
         <v>43453.45763888889</v>
       </c>
-    </row>
-    <row r="254" spans="1:15">
+      <c r="P253">
+        <v>0</v>
+      </c>
+      <c r="S253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:19">
       <c r="A254" s="2">
         <v>43454</v>
       </c>
@@ -12364,8 +13912,14 @@
       <c r="O254" s="3">
         <v>43454.45416666667</v>
       </c>
-    </row>
-    <row r="255" spans="1:15">
+      <c r="P254">
+        <v>0</v>
+      </c>
+      <c r="S254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:19">
       <c r="A255" s="2">
         <v>43455</v>
       </c>
@@ -12411,8 +13965,14 @@
       <c r="O255" s="3">
         <v>43455.4375</v>
       </c>
-    </row>
-    <row r="256" spans="1:15">
+      <c r="P255">
+        <v>0</v>
+      </c>
+      <c r="S255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:19">
       <c r="A256" s="2">
         <v>43458</v>
       </c>
@@ -12458,8 +14018,14 @@
       <c r="O256" s="3">
         <v>43458.44444444445</v>
       </c>
-    </row>
-    <row r="257" spans="1:15">
+      <c r="P256">
+        <v>0</v>
+      </c>
+      <c r="S256">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:19">
       <c r="A257" s="2">
         <v>43460</v>
       </c>
@@ -12505,8 +14071,14 @@
       <c r="O257" s="3">
         <v>43460.45763888889</v>
       </c>
-    </row>
-    <row r="258" spans="1:15">
+      <c r="P257">
+        <v>0</v>
+      </c>
+      <c r="S257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:19">
       <c r="A258" s="2">
         <v>43461</v>
       </c>
@@ -12552,8 +14124,14 @@
       <c r="O258" s="3">
         <v>43461.45972222222</v>
       </c>
-    </row>
-    <row r="259" spans="1:15">
+      <c r="P258">
+        <v>0</v>
+      </c>
+      <c r="S258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:19">
       <c r="A259" s="2">
         <v>43462</v>
       </c>
@@ -12599,8 +14177,14 @@
       <c r="O259" s="3">
         <v>43462.45486111111</v>
       </c>
-    </row>
-    <row r="260" spans="1:15">
+      <c r="P259">
+        <v>0</v>
+      </c>
+      <c r="S259">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="260" spans="1:19">
       <c r="A260" s="2">
         <v>43465</v>
       </c>
@@ -12645,6 +14229,12 @@
       </c>
       <c r="O260" s="3">
         <v>43465.45902777778</v>
+      </c>
+      <c r="P260">
+        <v>0</v>
+      </c>
+      <c r="S260">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>